<commit_message>
organizing files by lang
</commit_message>
<xml_diff>
--- a/DSA/problems_list.xlsx
+++ b/DSA/problems_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saakethm/Documents/Career/Interview_Prep/DSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86046FA6-3854-A74E-A736-6E3FED9B2E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5617B0-6492-E54B-B444-3CE98CFBD365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{4A3A3B0D-655C-AA46-B365-17CF081AA694}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{4A3A3B0D-655C-AA46-B365-17CF081AA694}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
   <si>
     <t>Problem Name</t>
   </si>
@@ -697,6 +697,29 @@
   </si>
   <si>
     <t>Array, Hash Table, String</t>
+  </si>
+  <si>
+    <t>use one stack to collect elements, for any pop/peek operation, move everything to second stack to get/remove top element, then move everything back.
+Then for any push operation, push to first stack
+Empty is easy (call on first stack)</t>
+  </si>
+  <si>
+    <t>push: make sure everything from s2 is in s1, then push to s1
+pop: move everything to s2. now top of stack is first in queue
+peek: same as pop!
+Empty: both are empty</t>
+  </si>
+  <si>
+    <t>push: O(N)
+pop: O(N)
+peek: O(N)
+Empty: O(1)</t>
+  </si>
+  <si>
+    <t>push: O(1)
+pop: O(1)
+peek: O(1)
+Empty: O(1)</t>
   </si>
 </sst>
 </file>
@@ -1117,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C4CD7D1-B787-ED4B-AC81-FB0452E28C73}">
   <dimension ref="B1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1156,7 +1179,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:9" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9" s="3" customFormat="1" ht="272" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1165,6 +1188,18 @@
       </c>
       <c r="D2" s="3" t="s">
         <v>28</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
updated cheatsheet first section
</commit_message>
<xml_diff>
--- a/DSA/problems_list.xlsx
+++ b/DSA/problems_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saakethm/Documents/Career/Interview_Prep/DSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104E335D-E46C-734E-A133-772345B6B7F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52DAF19-5DF1-034B-B75D-E94843796474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{4A3A3B0D-655C-AA46-B365-17CF081AA694}"/>
   </bookViews>
@@ -891,14 +891,14 @@
 Use a set to store each node, if referenced again then we're in a cycle.</t>
   </si>
   <si>
+    <t xml:space="preserve">O(N) </t>
+  </si>
+  <si>
+    <t>O(1), only two pointers!</t>
+  </si>
+  <si>
     <t>Floyd's Algorithm:
-Set two pointers. One moves incrementally by 1, the other moves twice as fast. Then if they ever meet at the same node, that guarantees there is a cycle (we can also calculate cycle length, but not necessary)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O(N) </t>
-  </si>
-  <si>
-    <t>O(1), only two pointers!</t>
+Set two pointers. One moves incrementally by 1, the other moves twice as fast. Then if they ever meet at the same node, that guarantees there is a cycle (we can also calculate cycle length by setting slow pointer to start and incrementing by 1 until they meet at cycle start which we can use to calculate length, but not necessary)</t>
   </si>
 </sst>
 </file>
@@ -1336,8 +1336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C4CD7D1-B787-ED4B-AC81-FB0452E28C73}">
   <dimension ref="B1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="125" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1479,7 +1479,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:9" s="3" customFormat="1" ht="188" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" s="3" customFormat="1" ht="205" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
@@ -1493,13 +1493,13 @@
         <v>73</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>24</v>

</xml_diff>